<commit_message>
Adição da rede de tarefas e atualização dos documentos
</commit_message>
<xml_diff>
--- a/Gerente/Gráfico de Gantt.xlsx
+++ b/Gerente/Gráfico de Gantt.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="68">
   <si>
     <t>MODELO DE GRÁFICO DE GANTT</t>
   </si>
@@ -192,31 +192,31 @@
     <t>Ikeda</t>
   </si>
   <si>
+    <t>2.14</t>
+  </si>
+  <si>
+    <t>Front-end</t>
+  </si>
+  <si>
+    <t>Cenedes</t>
+  </si>
+  <si>
+    <t>2.15</t>
+  </si>
+  <si>
+    <t>2.16</t>
+  </si>
+  <si>
+    <t>Ponto de Controle</t>
+  </si>
+  <si>
+    <t>Segunda Sprint (8-15)</t>
+  </si>
+  <si>
+    <t>Terceira Sprint (16-22)</t>
+  </si>
+  <si>
     <t>0 %</t>
-  </si>
-  <si>
-    <t>2.14</t>
-  </si>
-  <si>
-    <t>Front-end</t>
-  </si>
-  <si>
-    <t>Cenedes</t>
-  </si>
-  <si>
-    <t>2.15</t>
-  </si>
-  <si>
-    <t>2.16</t>
-  </si>
-  <si>
-    <t>Ponto de Controle</t>
-  </si>
-  <si>
-    <t>Segunda Sprint (8-15)</t>
-  </si>
-  <si>
-    <t>Terceira Sprint (16-22)</t>
   </si>
 </sst>
 </file>
@@ -921,17 +921,17 @@
     <xf borderId="10" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="11" fillId="0" fontId="24" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="24" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3227,8 +3227,8 @@
       <c r="G28" s="61">
         <v>6.0</v>
       </c>
-      <c r="H28" s="91" t="s">
-        <v>59</v>
+      <c r="H28" s="62">
+        <v>1.0</v>
       </c>
       <c r="I28" s="75"/>
       <c r="J28" s="76"/>
@@ -3295,13 +3295,13 @@
     <row r="29" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A29" s="57"/>
       <c r="B29" s="90" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="89" t="s">
+      <c r="D29" s="59" t="s">
         <v>61</v>
-      </c>
-      <c r="D29" s="59" t="s">
-        <v>62</v>
       </c>
       <c r="E29" s="60">
         <v>45567.0</v>
@@ -3312,8 +3312,8 @@
       <c r="G29" s="61">
         <v>6.0</v>
       </c>
-      <c r="H29" s="91" t="s">
-        <v>59</v>
+      <c r="H29" s="62">
+        <v>1.0</v>
       </c>
       <c r="I29" s="75"/>
       <c r="J29" s="76"/>
@@ -3380,7 +3380,7 @@
     <row r="30" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A30" s="57"/>
       <c r="B30" s="90" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" s="89" t="s">
         <v>51</v>
@@ -3397,8 +3397,8 @@
       <c r="G30" s="61">
         <v>3.0</v>
       </c>
-      <c r="H30" s="91" t="s">
-        <v>59</v>
+      <c r="H30" s="62">
+        <v>1.0</v>
       </c>
       <c r="I30" s="75"/>
       <c r="J30" s="76"/>
@@ -3465,10 +3465,10 @@
     <row r="31" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="57"/>
       <c r="B31" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="89" t="s">
         <v>64</v>
-      </c>
-      <c r="C31" s="89" t="s">
-        <v>65</v>
       </c>
       <c r="D31" s="59" t="s">
         <v>34</v>
@@ -3482,8 +3482,8 @@
       <c r="G31" s="61">
         <v>1.0</v>
       </c>
-      <c r="H31" s="91" t="s">
-        <v>59</v>
+      <c r="H31" s="62">
+        <v>1.0</v>
       </c>
       <c r="I31" s="75"/>
       <c r="J31" s="76"/>
@@ -3553,7 +3553,7 @@
         <v>3.0</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D32" s="51"/>
       <c r="E32" s="52"/>
@@ -3645,11 +3645,11 @@
       <c r="H33" s="62">
         <v>1.0</v>
       </c>
-      <c r="I33" s="92"/>
-      <c r="J33" s="93"/>
-      <c r="K33" s="94"/>
-      <c r="L33" s="94"/>
-      <c r="M33" s="94"/>
+      <c r="I33" s="91"/>
+      <c r="J33" s="92"/>
+      <c r="K33" s="93"/>
+      <c r="L33" s="93"/>
+      <c r="M33" s="93"/>
       <c r="N33" s="86"/>
       <c r="O33" s="86"/>
       <c r="P33" s="86"/>
@@ -3825,10 +3825,10 @@
       <c r="P35" s="86"/>
       <c r="Q35" s="86"/>
       <c r="R35" s="86"/>
-      <c r="S35" s="94"/>
-      <c r="T35" s="94"/>
-      <c r="U35" s="94"/>
-      <c r="V35" s="94"/>
+      <c r="S35" s="93"/>
+      <c r="T35" s="93"/>
+      <c r="U35" s="93"/>
+      <c r="V35" s="93"/>
       <c r="W35" s="77"/>
       <c r="X35" s="77"/>
       <c r="Y35" s="77"/>
@@ -3910,10 +3910,10 @@
       <c r="P36" s="86"/>
       <c r="Q36" s="86"/>
       <c r="R36" s="86"/>
-      <c r="S36" s="94"/>
-      <c r="T36" s="94"/>
-      <c r="U36" s="94"/>
-      <c r="V36" s="94"/>
+      <c r="S36" s="93"/>
+      <c r="T36" s="93"/>
+      <c r="U36" s="93"/>
+      <c r="V36" s="93"/>
       <c r="W36" s="77"/>
       <c r="X36" s="77"/>
       <c r="Y36" s="77"/>
@@ -3982,8 +3982,8 @@
       <c r="G37" s="61">
         <v>6.0</v>
       </c>
-      <c r="H37" s="91" t="s">
-        <v>59</v>
+      <c r="H37" s="62">
+        <v>1.0</v>
       </c>
       <c r="I37" s="75"/>
       <c r="J37" s="76"/>
@@ -3995,10 +3995,10 @@
       <c r="P37" s="86"/>
       <c r="Q37" s="86"/>
       <c r="R37" s="86"/>
-      <c r="S37" s="94"/>
-      <c r="T37" s="94"/>
-      <c r="U37" s="94"/>
-      <c r="V37" s="94"/>
+      <c r="S37" s="93"/>
+      <c r="T37" s="93"/>
+      <c r="U37" s="93"/>
+      <c r="V37" s="93"/>
       <c r="W37" s="77"/>
       <c r="X37" s="77"/>
       <c r="Y37" s="77"/>
@@ -4053,10 +4053,10 @@
         <v>45446.0</v>
       </c>
       <c r="C38" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="59" t="s">
         <v>61</v>
-      </c>
-      <c r="D38" s="59" t="s">
-        <v>62</v>
       </c>
       <c r="E38" s="60">
         <v>45575.0</v>
@@ -4067,8 +4067,8 @@
       <c r="G38" s="61">
         <v>6.0</v>
       </c>
-      <c r="H38" s="91" t="s">
-        <v>59</v>
+      <c r="H38" s="62">
+        <v>1.0</v>
       </c>
       <c r="I38" s="75"/>
       <c r="J38" s="76"/>
@@ -4080,10 +4080,10 @@
       <c r="P38" s="86"/>
       <c r="Q38" s="86"/>
       <c r="R38" s="86"/>
-      <c r="S38" s="94"/>
-      <c r="T38" s="94"/>
-      <c r="U38" s="94"/>
-      <c r="V38" s="94"/>
+      <c r="S38" s="93"/>
+      <c r="T38" s="93"/>
+      <c r="U38" s="93"/>
+      <c r="V38" s="93"/>
       <c r="W38" s="77"/>
       <c r="X38" s="77"/>
       <c r="Y38" s="77"/>
@@ -4152,8 +4152,8 @@
       <c r="G39" s="61">
         <v>3.0</v>
       </c>
-      <c r="H39" s="91" t="s">
-        <v>59</v>
+      <c r="H39" s="62">
+        <v>1.0</v>
       </c>
       <c r="I39" s="75"/>
       <c r="J39" s="76"/>
@@ -4165,10 +4165,10 @@
       <c r="P39" s="86"/>
       <c r="Q39" s="86"/>
       <c r="R39" s="86"/>
-      <c r="S39" s="94"/>
-      <c r="T39" s="94"/>
-      <c r="U39" s="94"/>
-      <c r="V39" s="94"/>
+      <c r="S39" s="93"/>
+      <c r="T39" s="93"/>
+      <c r="U39" s="93"/>
+      <c r="V39" s="93"/>
       <c r="W39" s="77"/>
       <c r="X39" s="77"/>
       <c r="Y39" s="77"/>
@@ -4223,7 +4223,7 @@
         <v>45507.0</v>
       </c>
       <c r="C40" s="89" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D40" s="59" t="s">
         <v>34</v>
@@ -4237,8 +4237,8 @@
       <c r="G40" s="61">
         <v>1.0</v>
       </c>
-      <c r="H40" s="91" t="s">
-        <v>59</v>
+      <c r="H40" s="62">
+        <v>1.0</v>
       </c>
       <c r="I40" s="75"/>
       <c r="J40" s="76"/>
@@ -4250,10 +4250,10 @@
       <c r="P40" s="86"/>
       <c r="Q40" s="86"/>
       <c r="R40" s="86"/>
-      <c r="S40" s="94"/>
-      <c r="T40" s="94"/>
-      <c r="U40" s="94"/>
-      <c r="V40" s="94"/>
+      <c r="S40" s="93"/>
+      <c r="T40" s="93"/>
+      <c r="U40" s="93"/>
+      <c r="V40" s="93"/>
       <c r="W40" s="77"/>
       <c r="X40" s="77"/>
       <c r="Y40" s="77"/>
@@ -4308,7 +4308,7 @@
         <v>4.0</v>
       </c>
       <c r="C41" s="50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D41" s="51"/>
       <c r="E41" s="52"/>
@@ -4400,11 +4400,11 @@
       <c r="H42" s="62">
         <v>1.0</v>
       </c>
-      <c r="I42" s="92"/>
-      <c r="J42" s="93"/>
-      <c r="K42" s="94"/>
-      <c r="L42" s="94"/>
-      <c r="M42" s="94"/>
+      <c r="I42" s="91"/>
+      <c r="J42" s="92"/>
+      <c r="K42" s="93"/>
+      <c r="L42" s="93"/>
+      <c r="M42" s="93"/>
       <c r="N42" s="67"/>
       <c r="O42" s="67"/>
       <c r="P42" s="67"/>
@@ -4580,10 +4580,10 @@
       <c r="P44" s="67"/>
       <c r="Q44" s="67"/>
       <c r="R44" s="67"/>
-      <c r="S44" s="94"/>
-      <c r="T44" s="94"/>
-      <c r="U44" s="94"/>
-      <c r="V44" s="94"/>
+      <c r="S44" s="93"/>
+      <c r="T44" s="93"/>
+      <c r="U44" s="93"/>
+      <c r="V44" s="93"/>
       <c r="W44" s="77"/>
       <c r="X44" s="77"/>
       <c r="Y44" s="77"/>
@@ -4665,10 +4665,10 @@
       <c r="P45" s="67"/>
       <c r="Q45" s="67"/>
       <c r="R45" s="67"/>
-      <c r="S45" s="94"/>
-      <c r="T45" s="94"/>
-      <c r="U45" s="94"/>
-      <c r="V45" s="94"/>
+      <c r="S45" s="93"/>
+      <c r="T45" s="93"/>
+      <c r="U45" s="93"/>
+      <c r="V45" s="93"/>
       <c r="W45" s="77"/>
       <c r="X45" s="77"/>
       <c r="Y45" s="77"/>
@@ -4737,8 +4737,8 @@
       <c r="G46" s="61">
         <v>6.0</v>
       </c>
-      <c r="H46" s="91" t="s">
-        <v>59</v>
+      <c r="H46" s="62">
+        <v>1.0</v>
       </c>
       <c r="I46" s="75"/>
       <c r="J46" s="76"/>
@@ -4750,10 +4750,10 @@
       <c r="P46" s="67"/>
       <c r="Q46" s="67"/>
       <c r="R46" s="67"/>
-      <c r="S46" s="94"/>
-      <c r="T46" s="94"/>
-      <c r="U46" s="94"/>
-      <c r="V46" s="94"/>
+      <c r="S46" s="93"/>
+      <c r="T46" s="93"/>
+      <c r="U46" s="93"/>
+      <c r="V46" s="93"/>
       <c r="W46" s="77"/>
       <c r="X46" s="77"/>
       <c r="Y46" s="77"/>
@@ -4808,10 +4808,10 @@
         <v>45447.0</v>
       </c>
       <c r="C47" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" s="59" t="s">
         <v>61</v>
-      </c>
-      <c r="D47" s="59" t="s">
-        <v>62</v>
       </c>
       <c r="E47" s="60">
         <v>45583.0</v>
@@ -4822,8 +4822,8 @@
       <c r="G47" s="61">
         <v>6.0</v>
       </c>
-      <c r="H47" s="91" t="s">
-        <v>59</v>
+      <c r="H47" s="94" t="s">
+        <v>67</v>
       </c>
       <c r="I47" s="75"/>
       <c r="J47" s="76"/>
@@ -4835,10 +4835,10 @@
       <c r="P47" s="67"/>
       <c r="Q47" s="67"/>
       <c r="R47" s="67"/>
-      <c r="S47" s="94"/>
-      <c r="T47" s="94"/>
-      <c r="U47" s="94"/>
-      <c r="V47" s="94"/>
+      <c r="S47" s="93"/>
+      <c r="T47" s="93"/>
+      <c r="U47" s="93"/>
+      <c r="V47" s="93"/>
       <c r="W47" s="77"/>
       <c r="X47" s="77"/>
       <c r="Y47" s="77"/>
@@ -4907,8 +4907,8 @@
       <c r="G48" s="61">
         <v>3.0</v>
       </c>
-      <c r="H48" s="91" t="s">
-        <v>59</v>
+      <c r="H48" s="94" t="s">
+        <v>67</v>
       </c>
       <c r="I48" s="75"/>
       <c r="J48" s="76"/>
@@ -4920,10 +4920,10 @@
       <c r="P48" s="67"/>
       <c r="Q48" s="67"/>
       <c r="R48" s="67"/>
-      <c r="S48" s="94"/>
-      <c r="T48" s="94"/>
-      <c r="U48" s="94"/>
-      <c r="V48" s="94"/>
+      <c r="S48" s="93"/>
+      <c r="T48" s="93"/>
+      <c r="U48" s="93"/>
+      <c r="V48" s="93"/>
       <c r="W48" s="77"/>
       <c r="X48" s="77"/>
       <c r="Y48" s="77"/>
@@ -4978,7 +4978,7 @@
         <v>45508.0</v>
       </c>
       <c r="C49" s="89" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D49" s="59" t="s">
         <v>34</v>
@@ -4992,8 +4992,8 @@
       <c r="G49" s="61">
         <v>1.0</v>
       </c>
-      <c r="H49" s="91" t="s">
-        <v>59</v>
+      <c r="H49" s="94" t="s">
+        <v>67</v>
       </c>
       <c r="I49" s="75"/>
       <c r="J49" s="76"/>
@@ -5005,10 +5005,10 @@
       <c r="P49" s="67"/>
       <c r="Q49" s="67"/>
       <c r="R49" s="67"/>
-      <c r="S49" s="94"/>
-      <c r="T49" s="94"/>
-      <c r="U49" s="94"/>
-      <c r="V49" s="94"/>
+      <c r="S49" s="93"/>
+      <c r="T49" s="93"/>
+      <c r="U49" s="93"/>
+      <c r="V49" s="93"/>
       <c r="W49" s="77"/>
       <c r="X49" s="77"/>
       <c r="Y49" s="77"/>

</xml_diff>

<commit_message>
Organização final de todos os documentos e codigo
</commit_message>
<xml_diff>
--- a/Gerente/Gráfico de Gantt.xlsx
+++ b/Gerente/Gráfico de Gantt.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="67">
   <si>
     <t>MODELO DE GRÁFICO DE GANTT</t>
   </si>
@@ -214,9 +214,6 @@
   </si>
   <si>
     <t>Terceira Sprint (16-22)</t>
-  </si>
-  <si>
-    <t>0 %</t>
   </si>
 </sst>
 </file>
@@ -667,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="94">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -929,9 +926,6 @@
     </xf>
     <xf borderId="12" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2055,43 +2049,43 @@
       <c r="K14" s="75"/>
       <c r="L14" s="65"/>
       <c r="M14" s="65"/>
-      <c r="N14" s="67"/>
-      <c r="O14" s="67"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="65"/>
       <c r="P14" s="67"/>
       <c r="Q14" s="67"/>
       <c r="R14" s="67"/>
-      <c r="S14" s="77"/>
-      <c r="T14" s="77"/>
+      <c r="S14" s="65"/>
+      <c r="T14" s="65"/>
       <c r="U14" s="77"/>
       <c r="V14" s="77"/>
       <c r="W14" s="77"/>
-      <c r="X14" s="77"/>
-      <c r="Y14" s="77"/>
+      <c r="X14" s="65"/>
+      <c r="Y14" s="65"/>
       <c r="Z14" s="77"/>
       <c r="AA14" s="77"/>
       <c r="AB14" s="77"/>
-      <c r="AC14" s="78"/>
-      <c r="AD14" s="78"/>
+      <c r="AC14" s="65"/>
+      <c r="AD14" s="65"/>
       <c r="AE14" s="78"/>
       <c r="AF14" s="78"/>
       <c r="AG14" s="78"/>
-      <c r="AH14" s="77"/>
-      <c r="AI14" s="77"/>
+      <c r="AH14" s="65"/>
+      <c r="AI14" s="65"/>
       <c r="AJ14" s="77"/>
       <c r="AK14" s="77"/>
       <c r="AL14" s="77"/>
-      <c r="AM14" s="77"/>
-      <c r="AN14" s="77"/>
+      <c r="AM14" s="65"/>
+      <c r="AN14" s="65"/>
       <c r="AO14" s="77"/>
       <c r="AP14" s="77"/>
       <c r="AQ14" s="77"/>
-      <c r="AR14" s="79"/>
-      <c r="AS14" s="79"/>
+      <c r="AR14" s="65"/>
+      <c r="AS14" s="65"/>
       <c r="AT14" s="79"/>
       <c r="AU14" s="79"/>
       <c r="AV14" s="79"/>
-      <c r="AW14" s="77"/>
-      <c r="AX14" s="77"/>
+      <c r="AW14" s="65"/>
+      <c r="AX14" s="65"/>
       <c r="AY14" s="77"/>
       <c r="AZ14" s="77"/>
       <c r="BA14" s="77"/>
@@ -4822,8 +4816,8 @@
       <c r="G47" s="61">
         <v>6.0</v>
       </c>
-      <c r="H47" s="94" t="s">
-        <v>67</v>
+      <c r="H47" s="62">
+        <v>1.0</v>
       </c>
       <c r="I47" s="75"/>
       <c r="J47" s="76"/>
@@ -4907,8 +4901,8 @@
       <c r="G48" s="61">
         <v>3.0</v>
       </c>
-      <c r="H48" s="94" t="s">
-        <v>67</v>
+      <c r="H48" s="62">
+        <v>1.0</v>
       </c>
       <c r="I48" s="75"/>
       <c r="J48" s="76"/>
@@ -4992,8 +4986,8 @@
       <c r="G49" s="61">
         <v>1.0</v>
       </c>
-      <c r="H49" s="94" t="s">
-        <v>67</v>
+      <c r="H49" s="62">
+        <v>1.0</v>
       </c>
       <c r="I49" s="75"/>
       <c r="J49" s="76"/>

</xml_diff>